<commit_message>
county data from NYT works
</commit_message>
<xml_diff>
--- a/Case Data Services/CDC data.xlsx
+++ b/Case Data Services/CDC data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/TeamPi-P2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/Team Pi/Case Data Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{EEA7F7AD-05AD-4146-BA41-DA0171A46592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE0C7CFC-A459-4DC4-8DB6-FA02C589179B}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{EEA7F7AD-05AD-4146-BA41-DA0171A46592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{227C049B-1CD4-4BEB-9743-956402E1ACC2}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="880" windowWidth="11780" windowHeight="9320" xr2:uid="{CBDAB3AD-8BDE-40AD-8699-8D8BB2D0D02B}"/>
+    <workbookView xWindow="1500" yWindow="810" windowWidth="10040" windowHeight="9340" xr2:uid="{CBDAB3AD-8BDE-40AD-8699-8D8BB2D0D02B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,15 +366,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>